<commit_message>
Modificaciones en web inicial. Silverio
</commit_message>
<xml_diff>
--- a/Market/Tareas.xlsx
+++ b/Market/Tareas.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Tareas" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Interfaces" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -298,7 +299,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -473,4 +474,30 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Multipleas cambios, adaptación clases a USER. Silverio
</commit_message>
<xml_diff>
--- a/Market/Tareas.xlsx
+++ b/Market/Tareas.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t xml:space="preserve">TAREAS</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t xml:space="preserve">ABEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actualizadas las clases anidades de User (User.DA) con los nuevos campos(apellido, teléfono y dirección). + constructor sin parámetros</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cambio de CP de String a Integer, User.DA ahora tiene parámetro que lee el tipo de usuario, Telefono es integer.</t>
   </si>
   <si>
     <t xml:space="preserve">PARA LAS VISTAS ESTOY USANDO BOOTSTRAP es un framework para pintar o maquetar HTML</t>
@@ -153,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -168,6 +174,13 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -194,16 +207,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -211,11 +240,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -296,160 +329,238 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="112"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="116.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="6" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="0" t="n">
+      <c r="B4" s="5"/>
+      <c r="C4" s="6" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="0" t="n">
+      <c r="B5" s="5"/>
+      <c r="C5" s="6" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="0" t="n">
+      <c r="B6" s="5"/>
+      <c r="C6" s="6" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="0" t="n">
+      <c r="B7" s="5"/>
+      <c r="C7" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="0" t="n">
+      <c r="B11" s="5"/>
+      <c r="C11" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="L11" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="0" t="n">
+      <c r="B12" s="5"/>
+      <c r="C12" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="L12" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="L13" s="3" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="L13" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="3"/>
-      <c r="L14" s="3" t="s">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="L14" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -461,7 +572,7 @@
       <formula1>"Responsables"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorTitle="Responsables asignados" operator="between" promptTitle="Responsable" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2:B17" type="list">
+    <dataValidation allowBlank="true" errorTitle="Responsables asignados" operator="between" promptTitle="Responsable" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2:B15 B28:B29" type="list">
       <formula1>$L$12:$L$14</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Detalle de autores, alertas, nombres sobre imagenes y opcion salir.
</commit_message>
<xml_diff>
--- a/Market/Tareas.xlsx
+++ b/Market/Tareas.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t xml:space="preserve">TAREAS</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t xml:space="preserve">Elimiar clases innecesarias → Coordinar con Abel (algunas ya eliminadas que no afectan a su trabajo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra: Introduccion en tabla nuevo carrito, ir metiendo item (importante CRUD), actulizar Estado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arreglar el problema de los Estados en la compra con la relación del carrito.</t>
   </si>
   <si>
     <t xml:space="preserve">PARA LAS VISTAS ESTOY USANDO BOOTSTRAP es un framework para pintar o maquetar HTML</t>
@@ -375,8 +381,8 @@
   </sheetPr>
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -556,7 +562,7 @@
       <c r="C18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="9"/>
@@ -591,12 +597,16 @@
       <c r="C23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6"/>
+      <c r="A24" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="B24" s="9"/>
       <c r="C24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6"/>
+      <c r="A25" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="B25" s="9"/>
       <c r="C25" s="6"/>
     </row>
@@ -612,14 +622,14 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>

</xml_diff>

<commit_message>
Cambios multiples en presentaciones. Añadido Javadoc
</commit_message>
<xml_diff>
--- a/Market/Tareas.xlsx
+++ b/Market/Tareas.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t xml:space="preserve">TAREAS</t>
   </si>
@@ -56,6 +56,9 @@
     <t xml:space="preserve">Función para obtener datos de un producto por ID(BL/DA)</t>
   </si>
   <si>
+    <t xml:space="preserve">Abel</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ofertas: Crear ofertas / Mostrar ofertas. Estas está relacionadas con los productos(INNER JOIN)</t>
   </si>
   <si>
@@ -87,6 +90,9 @@
   </si>
   <si>
     <t xml:space="preserve">¿por qué no usar la clase Producto que tiene un campo para almacenar la puntuación? Cambiado de esta forma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silverio</t>
   </si>
   <si>
     <t xml:space="preserve">Enseñarme la sintaxis para realizar una búsqueda que devuelva acorde a una ordenación de un campo dado.</t>
@@ -381,8 +387,8 @@
   </sheetPr>
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -459,35 +465,37 @@
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="C7" s="6" t="n">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="6" t="n">
@@ -499,7 +507,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="6" t="n">
@@ -511,7 +519,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
@@ -521,19 +529,19 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="6"/>
       <c r="L14" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>4</v>
@@ -542,70 +550,76 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="C17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="9"/>
       <c r="C19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="9"/>
+        <v>27</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="C21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="6"/>
@@ -622,14 +636,14 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="6"/>

</xml_diff>

<commit_message>
JavaDoc completado. Revisión Controllers, clases JAVA y controllers, Views
</commit_message>
<xml_diff>
--- a/Market/Tareas.xlsx
+++ b/Market/Tareas.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t xml:space="preserve">TAREAS</t>
   </si>
@@ -29,6 +29,9 @@
     <t xml:space="preserve">RESPONSABLE</t>
   </si>
   <si>
+    <t xml:space="preserve">RESPONSABLE 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">DURACION(días)</t>
   </si>
   <si>
@@ -41,10 +44,16 @@
     <t xml:space="preserve">Entrar con un Usuario y dejar el usuario ya en Session</t>
   </si>
   <si>
+    <t xml:space="preserve">ABEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silverio</t>
+  </si>
+  <si>
     <t xml:space="preserve">Crear un formulario con Bootstrap para crear usuarios</t>
   </si>
   <si>
-    <t xml:space="preserve">ABEL</t>
+    <t xml:space="preserve">Abel</t>
   </si>
   <si>
     <t xml:space="preserve">Funcionalidad en controller para crear usuario(Controller/BL/DA)</t>
@@ -56,9 +65,6 @@
     <t xml:space="preserve">Función para obtener datos de un producto por ID(BL/DA)</t>
   </si>
   <si>
-    <t xml:space="preserve">Abel</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ofertas: Crear ofertas / Mostrar ofertas. Estas está relacionadas con los productos(INNER JOIN)</t>
   </si>
   <si>
@@ -86,13 +92,10 @@
     <t xml:space="preserve"> Cambio de CP de String a Integer, User.DA ahora tiene parámetro que lee el tipo de usuario, Telefono es integer.</t>
   </si>
   <si>
-    <t xml:space="preserve">¿Qué es C11 en la búsqueda de los mejores productos? Clase Productos_BL</t>
+    <t xml:space="preserve">¿Qué es C11 en la búsqueda de los mejores productos? Clase Productos_BL, campo creado por la BBDD donde almacena resultado</t>
   </si>
   <si>
     <t xml:space="preserve">¿por qué no usar la clase Producto que tiene un campo para almacenar la puntuación? Cambiado de esta forma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silverio</t>
   </si>
   <si>
     <t xml:space="preserve">Enseñarme la sintaxis para realizar una búsqueda que devuelva acorde a una ordenación de un campo dado.</t>
@@ -163,7 +166,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,8 +181,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFB2B2B2"/>
+        <bgColor rgb="FFADC5E7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF72BF44"/>
-        <bgColor rgb="FF969696"/>
+        <bgColor rgb="FF339966"/>
       </patternFill>
     </fill>
     <fill>
@@ -216,17 +225,17 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -260,27 +269,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -288,23 +301,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -366,7 +375,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -385,281 +394,289 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="116.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="10.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="16.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.51"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="n">
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="7" t="n">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6" t="n">
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="7" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="5" t="s">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6" t="n">
+      <c r="D5" s="7" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="M13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="M14" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="6" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="L13" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="L14" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="6"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
+      <c r="B19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
+      <c r="B20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="6"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
+      <c r="B21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
+      <c r="B23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="6"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="6"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>33</v>
+      </c>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
+        <v>34</v>
+      </c>
+      <c r="D29" s="7"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" promptTitle="Responsable" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K6" type="none">
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="between" promptTitle="Responsable" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L6" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L11:L14" type="custom">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="M11:M14" type="custom">
       <formula1>"Responsables"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorTitle="Responsables asignados" operator="between" promptTitle="Responsable" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2:B15 B28:B29" type="list">
-      <formula1>$L$12:$L$14</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>